<commit_message>
Update Unit Test/XML Templates for onlineResources
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/Config_AB_XML_Publisher.xlsx
+++ b/FME_files/LOOKUP_TABLES/Config_AB_XML_Publisher.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="147">
   <si>
     <t>id</t>
   </si>
@@ -433,6 +433,33 @@
   </si>
   <si>
     <t>GMD_MDMETADATA;GMD_CONTACT;GMD_CITEDRESPONSIBLEPARTY;GMD_DISTRIBUTOR;GMD_DISTRIBUTIONFORMAT;GMD_KEYWORDS;GMD_REFERENCESYSTEMINFO;GMD_RESOURCEMAINTENANCE;GMD_TOPICCATEGORY;GMD_TRANSFEROPTIONS</t>
+  </si>
+  <si>
+    <t>online_resource_link</t>
+  </si>
+  <si>
+    <t>online_resource_protocol</t>
+  </si>
+  <si>
+    <t>contacts{}.postalcode</t>
+  </si>
+  <si>
+    <t>online_resource_description</t>
+  </si>
+  <si>
+    <t>online_resource_description_en</t>
+  </si>
+  <si>
+    <t>online_resource_description_other_lang_locale</t>
+  </si>
+  <si>
+    <t>online_resource_description_locale</t>
+  </si>
+  <si>
+    <t>online_resource_description_other_lang</t>
+  </si>
+  <si>
+    <t>online_resource_description_fr</t>
   </si>
 </sst>
 </file>
@@ -488,7 +515,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -750,13 +777,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.28515625" customWidth="1"/>
     <col min="2" max="2" width="73.7109375" customWidth="1"/>
@@ -1588,6 +1615,138 @@
         <v>79</v>
       </c>
     </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>138</v>
+      </c>
+      <c r="B76" t="s">
+        <v>138</v>
+      </c>
+      <c r="C76" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>139</v>
+      </c>
+      <c r="B77" t="s">
+        <v>139</v>
+      </c>
+      <c r="C77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>141</v>
+      </c>
+      <c r="B78" t="s">
+        <v>142</v>
+      </c>
+      <c r="C78" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>143</v>
+      </c>
+      <c r="B79" t="s">
+        <v>144</v>
+      </c>
+      <c r="C79" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>145</v>
+      </c>
+      <c r="B80" t="s">
+        <v>146</v>
+      </c>
+      <c r="C80" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" t="s">
+        <v>108</v>
+      </c>
+      <c r="C81" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>109</v>
+      </c>
+      <c r="B82" t="s">
+        <v>110</v>
+      </c>
+      <c r="C82" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>111</v>
+      </c>
+      <c r="B83" t="s">
+        <v>112</v>
+      </c>
+      <c r="C83" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>113</v>
+      </c>
+      <c r="B84" t="s">
+        <v>114</v>
+      </c>
+      <c r="C84" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>119</v>
+      </c>
+      <c r="B85" t="s">
+        <v>120</v>
+      </c>
+      <c r="C85" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>115</v>
+      </c>
+      <c r="B86" t="s">
+        <v>140</v>
+      </c>
+      <c r="C86" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>116</v>
+      </c>
+      <c r="B87" t="s">
+        <v>117</v>
+      </c>
+      <c r="C87" t="s">
+        <v>73</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add new attributes to reader / update Unit Tests
</commit_message>
<xml_diff>
--- a/FME_files/LOOKUP_TABLES/Config_AB_XML_Publisher.xlsx
+++ b/FME_files/LOOKUP_TABLES/Config_AB_XML_Publisher.xlsx
@@ -441,9 +441,6 @@
     <t>online_resource_protocol</t>
   </si>
   <si>
-    <t>contacts{}.postalcode</t>
-  </si>
-  <si>
     <t>online_resource_description</t>
   </si>
   <si>
@@ -460,6 +457,9 @@
   </si>
   <si>
     <t>online_resource_description_fr</t>
+  </si>
+  <si>
+    <t>contact_postal_code</t>
   </si>
 </sst>
 </file>
@@ -779,8 +779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1639,10 +1639,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
+        <v>140</v>
+      </c>
+      <c r="B78" t="s">
         <v>141</v>
-      </c>
-      <c r="B78" t="s">
-        <v>142</v>
       </c>
       <c r="C78" t="s">
         <v>73</v>
@@ -1650,10 +1650,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>142</v>
+      </c>
+      <c r="B79" t="s">
         <v>143</v>
-      </c>
-      <c r="B79" t="s">
-        <v>144</v>
       </c>
       <c r="C79" t="s">
         <v>73</v>
@@ -1661,10 +1661,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>144</v>
+      </c>
+      <c r="B80" t="s">
         <v>145</v>
-      </c>
-      <c r="B80" t="s">
-        <v>146</v>
       </c>
       <c r="C80" t="s">
         <v>73</v>
@@ -1727,10 +1727,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>115</v>
+        <v>146</v>
       </c>
       <c r="B86" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="C86" t="s">
         <v>73</v>

</xml_diff>